<commit_message>
Added vocabulary concept ids
</commit_message>
<xml_diff>
--- a/Conversion_from_v4/vocabulary conversion.xlsx
+++ b/Conversion_from_v4/vocabulary conversion.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="147">
   <si>
     <t>vocabulary_id</t>
   </si>
@@ -244,9 +244,6 @@
     <t>OMOP Measurement Type</t>
   </si>
   <si>
-    <t>International Currency Symbol</t>
-  </si>
-  <si>
     <t>vocabulary_code</t>
   </si>
   <si>
@@ -449,6 +446,21 @@
   </si>
   <si>
     <t>Version 1.8.2</t>
+  </si>
+  <si>
+    <t>Clinical Classifications Software for ICD-9-CM (HCUP)</t>
+  </si>
+  <si>
+    <t>Gemscript NHS dictionary of medicine and devices (NHS)</t>
+  </si>
+  <si>
+    <t>Hospital Episode Statistics Specialty (NHS)</t>
+  </si>
+  <si>
+    <t>International Currency Symbol (ISO 4217)</t>
+  </si>
+  <si>
+    <t>CONCEPT_ID</t>
   </si>
 </sst>
 </file>
@@ -456,8 +468,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="169" formatCode="yyyy\-dd\-mm"/>
-    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-dd\-mm"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -581,19 +593,19 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -891,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -907,12 +919,12 @@
     <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -923,8 +935,11 @@
       <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>0</v>
       </c>
@@ -941,8 +956,11 @@
         <f>LEN(B2)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
+      <c r="G2">
+        <v>44819096</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3">
         <v>1</v>
       </c>
@@ -950,20 +968,23 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F59" si="0">LEN(B3)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>44819097</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2</v>
       </c>
@@ -971,20 +992,23 @@
         <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>44819098</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>3</v>
       </c>
@@ -992,20 +1016,23 @@
         <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>44819099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1013,20 +1040,23 @@
         <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>44819100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1034,20 +1064,23 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>44819101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1055,20 +1088,23 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>44819102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1076,20 +1112,23 @@
         <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>44819103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1097,20 +1136,23 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>44819104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1118,20 +1160,23 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>44819105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1139,17 +1184,20 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <v>44819106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1157,38 +1205,44 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <v>44819107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <v>44819108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1196,20 +1250,23 @@
         <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <v>44819109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1217,10 +1274,10 @@
         <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E16" s="9">
         <v>40118</v>
@@ -1229,8 +1286,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>44819110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1238,20 +1298,23 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>137</v>
-      </c>
       <c r="F17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>44819111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1259,10 +1322,10 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E18" s="9">
         <v>41554</v>
@@ -1271,8 +1334,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1">
+      <c r="G18">
+        <v>44819112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1280,20 +1346,23 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1">
+      <c r="G19">
+        <v>44819113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1301,10 +1370,10 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E20" s="13">
         <v>39873</v>
@@ -1313,8 +1382,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1">
+      <c r="G20">
+        <v>44819114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1322,10 +1394,10 @@
         <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E21" s="11">
         <v>41445</v>
@@ -1334,8 +1406,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1">
+      <c r="G21">
+        <v>44819115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1343,10 +1418,10 @@
         <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E22" s="12">
         <v>41445</v>
@@ -1355,8 +1430,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1">
+      <c r="G22">
+        <v>44819116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1367,7 +1445,7 @@
         <v>68</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23" s="12">
         <v>41430</v>
@@ -1376,8 +1454,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>44819117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1385,20 +1466,23 @@
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1">
+      <c r="G24">
+        <v>44819118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1409,14 +1493,17 @@
         <v>16</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1">
+      <c r="G25">
+        <v>44819119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1">
       <c r="A26">
         <v>28</v>
       </c>
@@ -1424,20 +1511,23 @@
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1">
+      <c r="G26">
+        <v>44819120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1">
       <c r="A27">
         <v>31</v>
       </c>
@@ -1445,20 +1535,23 @@
         <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E27" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>141</v>
-      </c>
       <c r="F27">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1">
+      <c r="G27">
+        <v>44819121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1">
       <c r="A28">
         <v>32</v>
       </c>
@@ -1466,20 +1559,23 @@
         <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <v>44819122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>33</v>
       </c>
@@ -1487,17 +1583,20 @@
         <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <v>44819123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>34</v>
       </c>
@@ -1505,14 +1604,17 @@
         <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <v>44819124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>35</v>
       </c>
@@ -1520,14 +1622,17 @@
         <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <v>44819125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>36</v>
       </c>
@@ -1541,8 +1646,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <v>44819126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>37</v>
       </c>
@@ -1556,8 +1664,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <v>44819127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>38</v>
       </c>
@@ -1571,8 +1682,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <v>44819128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>39</v>
       </c>
@@ -1586,8 +1700,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <v>44819129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>40</v>
       </c>
@@ -1595,14 +1712,17 @@
         <v>25</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <v>44819130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>41</v>
       </c>
@@ -1610,14 +1730,17 @@
         <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <v>44819131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>42</v>
       </c>
@@ -1625,14 +1748,17 @@
         <v>27</v>
       </c>
       <c r="C38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <v>44819132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>43</v>
       </c>
@@ -1640,14 +1766,17 @@
         <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <v>44819133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>44</v>
       </c>
@@ -1655,14 +1784,17 @@
         <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <v>44819134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>45</v>
       </c>
@@ -1676,8 +1808,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41">
+        <v>44819135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>46</v>
       </c>
@@ -1685,14 +1820,17 @@
         <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42">
+        <v>44819136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>47</v>
       </c>
@@ -1700,14 +1838,17 @@
         <v>31</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43">
+        <v>44819137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>48</v>
       </c>
@@ -1715,14 +1856,17 @@
         <v>60</v>
       </c>
       <c r="C44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44">
+        <v>44819138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>49</v>
       </c>
@@ -1730,14 +1874,17 @@
         <v>61</v>
       </c>
       <c r="C45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <v>44819139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>50</v>
       </c>
@@ -1745,14 +1892,17 @@
         <v>62</v>
       </c>
       <c r="C46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46">
+        <v>44819140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>53</v>
       </c>
@@ -1760,14 +1910,17 @@
         <v>63</v>
       </c>
       <c r="C47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <v>44819141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>54</v>
       </c>
@@ -1775,14 +1928,17 @@
         <v>32</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48">
+        <v>44819142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>55</v>
       </c>
@@ -1790,14 +1946,17 @@
         <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49">
+        <v>44819143</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>56</v>
       </c>
@@ -1805,14 +1964,17 @@
         <v>33</v>
       </c>
       <c r="C50" t="s">
-        <v>33</v>
+        <v>143</v>
       </c>
       <c r="F50">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50">
+        <v>44819144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>57</v>
       </c>
@@ -1820,14 +1982,17 @@
         <v>34</v>
       </c>
       <c r="C51" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="F51">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51">
+        <v>44819145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>58</v>
       </c>
@@ -1841,8 +2006,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52">
+        <v>44819146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>59</v>
       </c>
@@ -1856,8 +2024,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53">
+        <v>44819147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>60</v>
       </c>
@@ -1871,13 +2042,16 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54">
+        <v>44819148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C55" t="s">
         <v>38</v>
@@ -1886,8 +2060,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55">
+        <v>44819149</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>62</v>
       </c>
@@ -1901,8 +2078,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56">
+        <v>44819150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>63</v>
       </c>
@@ -1916,13 +2096,16 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57">
+        <v>44819151</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C58" t="s">
         <v>73</v>
@@ -1931,8 +2114,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58">
+        <v>44819152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>65</v>
       </c>
@@ -1940,11 +2126,14 @@
         <v>72</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>145</v>
       </c>
       <c r="F59">
         <f t="shared" si="0"/>
         <v>8</v>
+      </c>
+      <c r="G59">
+        <v>44819153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Production version of V5.0 converted from 4.5
</commit_message>
<xml_diff>
--- a/Conversion_from_v4/vocabulary conversion.xlsx
+++ b/Conversion_from_v4/vocabulary conversion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="21360" windowHeight="10080"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="18660" windowHeight="10080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,14 @@
   </sheets>
   <definedNames>
     <definedName name="OLE_LINK1" localSheetId="0">Sheet1!$D$26</definedName>
-    <definedName name="OLE_LINK2" localSheetId="0">Sheet1!$E$26</definedName>
+    <definedName name="OLE_LINK2" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="175">
   <si>
     <t>vocabulary_id</t>
   </si>
@@ -34,9 +34,6 @@
     <t>vocabulary_version</t>
   </si>
   <si>
-    <t>OMOP Vocabulary v4.5 10-Sep-2014</t>
-  </si>
-  <si>
     <t>HCPCS</t>
   </si>
   <si>
@@ -229,9 +226,6 @@
     <t>WHO Anatomic Therapeutic Chemical Classification</t>
   </si>
   <si>
-    <t>v5.0 10-Sep-2014</t>
-  </si>
-  <si>
     <t>Device Type</t>
   </si>
   <si>
@@ -361,9 +355,6 @@
     <t>Medicare provider/supplier specialty codes (CMS)</t>
   </si>
   <si>
-    <t>LOINC Multidimensional Classification (Regenstrief Institute)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Structured Product Labeling (FDA)</t>
   </si>
   <si>
@@ -433,9 +424,6 @@
     <t>Version 16.1</t>
   </si>
   <si>
-    <t>April 2014 RELEASE</t>
-  </si>
-  <si>
     <t>Codes extracted from GPRD database, courtesy of GSK</t>
   </si>
   <si>
@@ -461,6 +449,102 @@
   </si>
   <si>
     <t>CONCEPT_ID</t>
+  </si>
+  <si>
+    <t>OMOP Vocabulary</t>
+  </si>
+  <si>
+    <t>v5.0 2014-10-15</t>
+  </si>
+  <si>
+    <t>National Patient-Centered Clinical Research Network (PCORI)</t>
+  </si>
+  <si>
+    <t>http://www.iso.org/iso/home/standards/currency_codes.htm</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>OMOP Relationship</t>
+  </si>
+  <si>
+    <t>Vocabulary</t>
+  </si>
+  <si>
+    <t>Concept Class</t>
+  </si>
+  <si>
+    <t>OMOP Concept Class</t>
+  </si>
+  <si>
+    <t>Cohort Type</t>
+  </si>
+  <si>
+    <t>OMOP Cohort Type</t>
+  </si>
+  <si>
+    <t>http://www.cms.gov/Medicare/Medicare-Fee-for-Service-Payment/AcuteInpatientPPS/Acute-Inpatient-Files-for-Download.html</t>
+  </si>
+  <si>
+    <t>http://www.cdc.gov/nchs/icd/icd10cm.htm</t>
+  </si>
+  <si>
+    <t>http://www.cms.gov/Medicare/Coding/ICD10/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cms.gov/Medicare/Medicare-Fee-for-Service-Payment/HospitalOutpatientPPS/Hospital-Outpatient-Regulations-and-Notices.html</t>
+  </si>
+  <si>
+    <t>http://www.mpca.net/?page=ERC_finance</t>
+  </si>
+  <si>
+    <t>2010 Release</t>
+  </si>
+  <si>
+    <t>http://www.nucc.org/index.php?option=com_content&amp;view=article&amp;id=107&amp;Itemid=132</t>
+  </si>
+  <si>
+    <t>http://www.cms.gov/Medicare/Provider-Enrollment-and-Certification/MedicareProviderSupEnroll/Taxonomy.html</t>
+  </si>
+  <si>
+    <t>http://loinc.org/downloads/accessory-files</t>
+  </si>
+  <si>
+    <t>LOINC Multiaxial Hierarchy (Regenstrief Institute)</t>
+  </si>
+  <si>
+    <t>http://www.fda.gov/Drugs/InformationOnDrugs/ucm142438.htm</t>
+  </si>
+  <si>
+    <t>http://www.hcup-us.ahrq.gov/toolssoftware/ccs/ccs.jsp#download</t>
+  </si>
+  <si>
+    <t>http://systems.hscic.gov.uk/data/clinicalcoding/codingstandards/opcs4</t>
+  </si>
+  <si>
+    <t>April 2014 Release</t>
+  </si>
+  <si>
+    <t>Codes extracted from GPRD database, courtesy of J&amp;J</t>
+  </si>
+  <si>
+    <t>2013 Release</t>
+  </si>
+  <si>
+    <t>Not implemented yet</t>
+  </si>
+  <si>
+    <t>http://www.datadictionary.nhs.uk/data_dictionary/attributes/m/main_specialty_code_de.asp?shownav=0</t>
+  </si>
+  <si>
+    <t>ICD10</t>
+  </si>
+  <si>
+    <t>http://www.who.int/classifications/icd/icdonlineversions/en/</t>
+  </si>
+  <si>
+    <t>International Classification of Diseases, 10th Revision, (WHO)</t>
   </si>
 </sst>
 </file>
@@ -471,32 +555,13 @@
     <numFmt numFmtId="164" formatCode="yyyy\-dd\-mm"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -507,7 +572,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -515,102 +580,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -903,28 +883,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76.140625" customWidth="1"/>
-    <col min="4" max="4" width="137.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" customWidth="1"/>
+    <col min="4" max="4" width="53.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -932,1208 +911,1227 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="F1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>69</v>
+        <v>143</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="F2">
-        <f>LEN(B2)</f>
-        <v>4</v>
-      </c>
-      <c r="G2">
         <v>44819096</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1">
+    <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>128</v>
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F59" si="0">LEN(B3)</f>
-        <v>6</v>
-      </c>
-      <c r="G3">
         <v>44819097</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>117</v>
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G4">
         <v>44819098</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>117</v>
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G5">
         <v>44819099</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>128</v>
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G6">
         <v>44819100</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>128</v>
+        <v>82</v>
+      </c>
+      <c r="D7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G7">
         <v>44819101</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>129</v>
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G8">
         <v>44819102</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>130</v>
+        <v>84</v>
+      </c>
+      <c r="D9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G9">
         <v>44819103</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>131</v>
+        <v>85</v>
+      </c>
+      <c r="D10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G10">
         <v>44819104</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>132</v>
+        <v>86</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G11">
         <v>44819105</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>119</v>
+        <v>80</v>
+      </c>
+      <c r="D12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="1">
+        <v>40664</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G12">
         <v>44819106</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>141</v>
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G13">
         <v>44819107</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>120</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" s="1"/>
       <c r="F14">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G14">
         <v>44819108</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>121</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>133</v>
+        <v>118</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G15">
         <v>44819109</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="E16" s="9">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>131</v>
+      </c>
+      <c r="E16" s="1">
         <v>40118</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="G16">
         <v>44819110</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>136</v>
+        <v>90</v>
+      </c>
+      <c r="D17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G17">
         <v>44819111</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E18" s="9">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="1">
         <v>41554</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G18">
         <v>44819112</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1">
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>137</v>
+        <v>92</v>
+      </c>
+      <c r="D19" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G19">
         <v>44819113</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1">
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E20" s="13">
+        <v>93</v>
+      </c>
+      <c r="D20" t="s">
+        <v>134</v>
+      </c>
+      <c r="E20" s="2">
         <v>39873</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G20">
         <v>44819114</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1">
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E21" s="11">
+        <v>94</v>
+      </c>
+      <c r="D21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="1">
         <v>41445</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G21">
         <v>44819115</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1">
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E22" s="12">
+        <v>95</v>
+      </c>
+      <c r="D22" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="1">
         <v>41445</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G22">
         <v>44819116</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1">
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E23" s="12">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="1">
         <v>41430</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G23">
         <v>44819117</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>131</v>
+        <v>96</v>
+      </c>
+      <c r="D24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" s="1">
+        <v>41430</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G24">
         <v>44819118</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1">
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>120</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" s="1"/>
       <c r="F25">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G25">
         <v>44819119</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1">
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>131</v>
+        <v>97</v>
+      </c>
+      <c r="D26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G26">
         <v>44819120</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1">
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>140</v>
+        <v>98</v>
+      </c>
+      <c r="D27" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G27">
         <v>44819121</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1">
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>101</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>131</v>
+        <v>99</v>
+      </c>
+      <c r="D28" t="s">
+        <v>121</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G28">
         <v>44819122</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>120</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="E29" s="1"/>
       <c r="F29">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G29">
         <v>44819123</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>172</v>
       </c>
       <c r="C30" t="s">
-        <v>103</v>
+        <v>174</v>
+      </c>
+      <c r="D30" t="s">
+        <v>173</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="G30">
         <v>44819124</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="D31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E31" s="1">
+        <v>40702</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G31">
         <v>44819125</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D32" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32" s="1"/>
       <c r="F32">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G32">
         <v>44819126</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33" s="1"/>
       <c r="F33">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="G33">
         <v>44819127</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D34" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="1"/>
       <c r="F34">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="G34">
         <v>44819128</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D35" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" s="1"/>
       <c r="F35">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="G35">
         <v>44819129</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+      <c r="D36" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" s="1">
+        <v>40592</v>
       </c>
       <c r="F36">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G36">
         <v>44819130</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>106</v>
+        <v>104</v>
+      </c>
+      <c r="D37" t="s">
+        <v>154</v>
+      </c>
+      <c r="E37" s="1">
+        <v>41426</v>
       </c>
       <c r="F37">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G37">
         <v>44819131</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="D38" t="s">
+        <v>157</v>
+      </c>
+      <c r="E38" s="1">
+        <v>40814</v>
       </c>
       <c r="F38">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G38">
         <v>44819132</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" t="s">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="D39" t="s">
+        <v>158</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="F39">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="G39">
         <v>44819133</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="D40" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" s="1"/>
       <c r="F40">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G40">
         <v>44819134</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D41" t="s">
+        <v>117</v>
+      </c>
+      <c r="E41" s="1"/>
       <c r="F41">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G41">
         <v>44819135</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C42" t="s">
-        <v>110</v>
+        <v>108</v>
+      </c>
+      <c r="D42" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="F42">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G42">
         <v>44819136</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>109</v>
+      </c>
+      <c r="D43" t="s">
+        <v>160</v>
+      </c>
+      <c r="E43" s="1">
+        <v>41281</v>
       </c>
       <c r="F43">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G43">
         <v>44819137</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
-        <v>112</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="D44" t="s">
+        <v>161</v>
+      </c>
+      <c r="E44" s="1"/>
       <c r="F44">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G44">
         <v>44819138</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C45" t="s">
-        <v>113</v>
+        <v>163</v>
+      </c>
+      <c r="D45" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45" t="s">
+        <v>126</v>
       </c>
       <c r="F45">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="G45">
         <v>44819139</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" t="s">
-        <v>114</v>
+        <v>111</v>
+      </c>
+      <c r="D46" t="s">
+        <v>164</v>
+      </c>
+      <c r="E46" s="1">
+        <v>41549</v>
       </c>
       <c r="F46">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G46">
         <v>44819140</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="D47" t="s">
+        <v>112</v>
+      </c>
+      <c r="E47" s="1">
+        <v>40780</v>
       </c>
       <c r="F47">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G47">
         <v>44819141</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C48" t="s">
-        <v>142</v>
+        <v>138</v>
+      </c>
+      <c r="D48" t="s">
+        <v>165</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="F48">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G48">
         <v>44819142</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" t="s">
-        <v>81</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D49" t="s">
+        <v>166</v>
+      </c>
+      <c r="E49" s="1"/>
       <c r="F49">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G49">
         <v>44819143</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C50" t="s">
-        <v>143</v>
+        <v>139</v>
+      </c>
+      <c r="D50" t="s">
+        <v>168</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="F50">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G50">
         <v>44819144</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:6">
       <c r="A51">
         <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C51" t="s">
-        <v>144</v>
+        <v>140</v>
+      </c>
+      <c r="D51" t="s">
+        <v>171</v>
+      </c>
+      <c r="E51" t="s">
+        <v>170</v>
       </c>
       <c r="F51">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="G51">
         <v>44819145</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:6">
       <c r="A52">
         <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C52" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D52" t="s">
+        <v>117</v>
+      </c>
+      <c r="E52" s="1"/>
       <c r="F52">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G52">
         <v>44819146</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:6">
       <c r="A53">
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D53" t="s">
+        <v>117</v>
+      </c>
+      <c r="E53" s="1"/>
       <c r="F53">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G53">
         <v>44819147</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:6">
       <c r="A54">
         <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C54" t="s">
-        <v>37</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="D54" t="s">
+        <v>117</v>
+      </c>
+      <c r="E54" s="1"/>
       <c r="F54">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="G54">
         <v>44819148</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:6">
       <c r="A55">
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C55" t="s">
-        <v>38</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D55" t="s">
+        <v>117</v>
+      </c>
+      <c r="E55" s="1"/>
       <c r="F55">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="G55">
         <v>44819149</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C56" t="s">
-        <v>39</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D56" t="s">
+        <v>117</v>
+      </c>
+      <c r="E56" s="1"/>
       <c r="F56">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G56">
         <v>44819150</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:6">
       <c r="A57">
         <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C57" t="s">
-        <v>71</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="D57" t="s">
+        <v>117</v>
+      </c>
+      <c r="E57" s="1"/>
       <c r="F57">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="G57">
         <v>44819151</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:6">
       <c r="A58">
         <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C58" t="s">
-        <v>73</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="D58" t="s">
+        <v>117</v>
+      </c>
+      <c r="E58" s="1"/>
       <c r="F58">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G58">
         <v>44819152</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C59" t="s">
-        <v>145</v>
+        <v>141</v>
+      </c>
+      <c r="D59" t="s">
+        <v>146</v>
+      </c>
+      <c r="E59" s="3">
+        <v>2008</v>
       </c>
       <c r="F59">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G59">
         <v>44819153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
+        <v>66</v>
+      </c>
+      <c r="B60" t="s">
+        <v>147</v>
+      </c>
+      <c r="C60" t="s">
+        <v>148</v>
+      </c>
+      <c r="D60" t="s">
+        <v>117</v>
+      </c>
+      <c r="E60" s="1"/>
+      <c r="F60">
+        <v>44819235</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
+        <v>67</v>
+      </c>
+      <c r="B61" t="s">
+        <v>149</v>
+      </c>
+      <c r="C61" t="s">
+        <v>143</v>
+      </c>
+      <c r="D61" t="s">
+        <v>117</v>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="F61">
+        <v>44819232</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
+        <v>68</v>
+      </c>
+      <c r="B62" t="s">
+        <v>150</v>
+      </c>
+      <c r="C62" t="s">
+        <v>151</v>
+      </c>
+      <c r="D62" t="s">
+        <v>117</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62">
+        <v>44819233</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
+        <v>69</v>
+      </c>
+      <c r="B63" t="s">
+        <v>152</v>
+      </c>
+      <c r="C63" t="s">
+        <v>153</v>
+      </c>
+      <c r="D63" t="s">
+        <v>117</v>
+      </c>
+      <c r="E63" s="1"/>
+      <c r="F63">
+        <v>44819234</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64">
+        <v>70</v>
+      </c>
+      <c r="B64" t="s">
+        <v>51</v>
+      </c>
+      <c r="C64" t="s">
+        <v>101</v>
+      </c>
+      <c r="D64" t="s">
+        <v>155</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F64">
+        <v>44819124</v>
       </c>
     </row>
   </sheetData>
@@ -2146,23 +2144,16 @@
     <hyperlink ref="D4" r:id="rId6"/>
     <hyperlink ref="D3" r:id="rId7"/>
     <hyperlink ref="D9" r:id="rId8"/>
-    <hyperlink ref="E9" r:id="rId9" display="http://download.nlm.nih.gov/umls/kss/rxnorm/RxNorm_full_07072014.zip"/>
-    <hyperlink ref="E10:E11" r:id="rId10" display="http://download.nlm.nih.gov/umls/kss/rxnorm/RxNorm_full_07072014.zip"/>
-    <hyperlink ref="D16" r:id="rId11" display="http://www.cms.gov/Medicare/Medicare-Fee-for-Service-Payment/PhysicianFeeSched/downloads/Website_POS_database.pdf"/>
-    <hyperlink ref="D17" r:id="rId12"/>
-    <hyperlink ref="D18" r:id="rId13"/>
-    <hyperlink ref="D19" r:id="rId14"/>
-    <hyperlink ref="D26" r:id="rId15"/>
-    <hyperlink ref="D27" r:id="rId16"/>
-    <hyperlink ref="D28" r:id="rId17"/>
-    <hyperlink ref="D24" r:id="rId18"/>
-    <hyperlink ref="E27" r:id="rId19" display="http://download.nlm.nih.gov/umls/kss/rxnorm/RxNorm_full_07072014.zip"/>
-    <hyperlink ref="E26" r:id="rId20" display="http://download.nlm.nih.gov/umls/kss/rxnorm/RxNorm_full_07072014.zip"/>
-    <hyperlink ref="E28" r:id="rId21" display="http://download.nlm.nih.gov/umls/kss/rxnorm/RxNorm_full_07072014.zip"/>
-    <hyperlink ref="E24" r:id="rId22" display="http://download.nlm.nih.gov/umls/kss/rxnorm/RxNorm_full_07072014.zip"/>
+    <hyperlink ref="D16" r:id="rId9" display="http://www.cms.gov/Medicare/Medicare-Fee-for-Service-Payment/PhysicianFeeSched/downloads/Website_POS_database.pdf"/>
+    <hyperlink ref="D17" r:id="rId10"/>
+    <hyperlink ref="D18" r:id="rId11"/>
+    <hyperlink ref="D19" r:id="rId12"/>
+    <hyperlink ref="D27" r:id="rId13"/>
+    <hyperlink ref="D28" r:id="rId14"/>
+    <hyperlink ref="D24" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 

</xml_diff>